<commit_message>
Add Excel file with conflict matrix v0.6
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.6.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerjan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerjan/Workshop/TrafficLightController/conflictMatrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDEBD4E-A0C1-E04A-B5B7-27DC59889C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2895E-F961-AF4C-A374-52EA9CBD5F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="940" windowWidth="25040" windowHeight="13700" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="300" yWindow="920" windowWidth="25040" windowHeight="13700" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,8 +90,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,28 +139,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -164,32 +169,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,92 +498,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="13"/>
-      <c r="B1" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E1" s="1">
-        <v>6.1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>7.1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="H1" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="I1" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="J1" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="K1" s="1">
-        <v>12.1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>86.1</v>
-      </c>
-      <c r="M1" s="1">
-        <v>35.1</v>
-      </c>
-      <c r="N1" s="1">
-        <v>26.1</v>
-      </c>
-      <c r="O1" s="1">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P1" s="1">
-        <v>88.1</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R1" s="1">
-        <v>28.1</v>
-      </c>
-      <c r="S1" s="1">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T1" s="1">
-        <v>31.2</v>
-      </c>
-      <c r="U1" s="2">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1">
+      <c r="A1" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="D1" s="5">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E1" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="F1" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="G1" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="H1" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="I1" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="J1" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="K1" s="4">
+        <v>12.1</v>
+      </c>
+      <c r="L1" s="6">
+        <v>86.1</v>
+      </c>
+      <c r="M1" s="6">
+        <v>35.1</v>
+      </c>
+      <c r="N1" s="6">
+        <v>26.1</v>
+      </c>
+      <c r="O1" s="6">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P1" s="7">
+        <v>88.1</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R1" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="S1" s="7">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T1" s="7">
+        <v>31.2</v>
+      </c>
+      <c r="U1" s="7">
+        <v>22</v>
+      </c>
+      <c r="V1" s="7">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="A2" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="3">
         <v>2.1</v>
       </c>
       <c r="D2" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>6.1</v>
       </c>
       <c r="F2" s="4">
@@ -599,43 +602,43 @@
       <c r="H2" s="5">
         <v>9.1</v>
       </c>
-      <c r="I2" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="J2" s="4">
-        <v>11.1</v>
-      </c>
-      <c r="K2" s="4">
-        <v>12.1</v>
-      </c>
-      <c r="L2" s="6">
-        <v>86.1</v>
-      </c>
-      <c r="M2" s="6">
-        <v>35.1</v>
-      </c>
-      <c r="N2" s="6">
-        <v>26.1</v>
-      </c>
-      <c r="O2" s="6">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P2" s="7">
-        <v>88.1</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R2" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="S2" s="7">
+      <c r="I2" s="5">
+        <v>10.1</v>
+      </c>
+      <c r="J2" s="5">
+        <v>11.1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>12.1</v>
+      </c>
+      <c r="L2" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="M2" s="7">
+        <v>35.1</v>
+      </c>
+      <c r="N2" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="O2" s="7">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P2" s="6">
+        <v>88.1</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R2" s="6">
+        <v>28.1</v>
+      </c>
+      <c r="S2" s="6">
         <v>38.200000000000003</v>
       </c>
       <c r="T2" s="7">
         <v>31.2</v>
       </c>
-      <c r="U2" s="8">
+      <c r="U2" s="7">
         <v>22</v>
       </c>
       <c r="V2" s="7">
@@ -643,67 +646,67 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="A3" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E3" s="4">
         <v>6.1</v>
       </c>
       <c r="F3" s="4">
         <v>7.1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>8.1</v>
       </c>
       <c r="H3" s="5">
         <v>9.1</v>
       </c>
-      <c r="I3" s="5">
-        <v>10.1</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="I3" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="J3" s="4">
         <v>11.1</v>
       </c>
       <c r="K3" s="5">
         <v>12.1</v>
       </c>
-      <c r="L3" s="7">
-        <v>86.1</v>
-      </c>
-      <c r="M3" s="7">
-        <v>35.1</v>
-      </c>
-      <c r="N3" s="7">
-        <v>26.1</v>
-      </c>
-      <c r="O3" s="7">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P3" s="6">
-        <v>88.1</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R3" s="6">
-        <v>28.1</v>
-      </c>
-      <c r="S3" s="6">
+      <c r="L3" s="6">
+        <v>86.1</v>
+      </c>
+      <c r="M3" s="6">
+        <v>35.1</v>
+      </c>
+      <c r="N3" s="6">
+        <v>26.1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P3" s="7">
+        <v>88.1</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R3" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="S3" s="7">
         <v>38.200000000000003</v>
       </c>
       <c r="T3" s="7">
         <v>31.2</v>
       </c>
-      <c r="U3" s="8">
+      <c r="U3" s="7">
         <v>22</v>
       </c>
       <c r="V3" s="7">
@@ -711,19 +714,19 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="B4" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="5">
         <v>2.1</v>
       </c>
-      <c r="D4" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E4" s="3">
         <v>6.1</v>
       </c>
       <c r="F4" s="4">
@@ -735,81 +738,81 @@
       <c r="H4" s="5">
         <v>9.1</v>
       </c>
-      <c r="I4" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" s="5">
+        <v>10.1</v>
+      </c>
+      <c r="J4" s="5">
         <v>11.1</v>
       </c>
       <c r="K4" s="5">
         <v>12.1</v>
       </c>
-      <c r="L4" s="6">
-        <v>86.1</v>
-      </c>
-      <c r="M4" s="6">
-        <v>35.1</v>
-      </c>
-      <c r="N4" s="6">
-        <v>26.1</v>
-      </c>
-      <c r="O4" s="6">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P4" s="7">
-        <v>88.1</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R4" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="S4" s="7">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T4" s="7">
-        <v>31.2</v>
-      </c>
-      <c r="U4" s="8">
-        <v>22</v>
-      </c>
-      <c r="V4" s="7">
+      <c r="L4" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>35.1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>26.1</v>
+      </c>
+      <c r="O4" s="7">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P4" s="6">
+        <v>88.1</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R4" s="6">
+        <v>28.1</v>
+      </c>
+      <c r="S4" s="6">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T4" s="6">
+        <v>31.2</v>
+      </c>
+      <c r="U4" s="6">
+        <v>22</v>
+      </c>
+      <c r="V4" s="6">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>6.1</v>
+      <c r="A5" s="2">
+        <v>7.1</v>
       </c>
       <c r="B5" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>2.1</v>
       </c>
       <c r="D5" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E5" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="F5" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>8.1</v>
-      </c>
-      <c r="H5" s="5">
-        <v>9.1</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="E5" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="I5" s="4">
         <v>10.1</v>
       </c>
       <c r="J5" s="5">
         <v>11.1</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>12.1</v>
       </c>
       <c r="L5" s="7">
@@ -839,7 +842,7 @@
       <c r="T5" s="6">
         <v>31.2</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="6">
         <v>22</v>
       </c>
       <c r="V5" s="6">
@@ -847,8 +850,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>7.1</v>
+      <c r="A6" s="2">
+        <v>8.1</v>
       </c>
       <c r="B6" s="4">
         <v>1.1000000000000001</v>
@@ -856,16 +859,16 @@
       <c r="C6" s="4">
         <v>2.1</v>
       </c>
-      <c r="D6" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E6" s="4">
-        <v>6.1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="D6" s="5">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="G6" s="3">
         <v>8.1</v>
       </c>
       <c r="H6" s="4">
@@ -877,7 +880,7 @@
       <c r="J6" s="5">
         <v>11.1</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>12.1</v>
       </c>
       <c r="L6" s="7">
@@ -904,24 +907,24 @@
       <c r="S6" s="6">
         <v>38.200000000000003</v>
       </c>
-      <c r="T6" s="6">
-        <v>31.2</v>
-      </c>
-      <c r="U6" s="9">
-        <v>22</v>
-      </c>
-      <c r="V6" s="6">
+      <c r="T6" s="7">
+        <v>31.2</v>
+      </c>
+      <c r="U6" s="7">
+        <v>22</v>
+      </c>
+      <c r="V6" s="7">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="A7" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7" s="5">
         <v>2.1</v>
       </c>
       <c r="D7" s="5">
@@ -933,10 +936,10 @@
       <c r="F7" s="4">
         <v>7.1</v>
       </c>
-      <c r="G7" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="H7" s="3">
         <v>9.1</v>
       </c>
       <c r="I7" s="4">
@@ -960,39 +963,39 @@
       <c r="O7" s="7">
         <v>36.200000000000003</v>
       </c>
-      <c r="P7" s="6">
-        <v>88.1</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R7" s="6">
-        <v>28.1</v>
-      </c>
-      <c r="S7" s="6">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T7" s="7">
-        <v>31.2</v>
-      </c>
-      <c r="U7" s="8">
-        <v>22</v>
-      </c>
-      <c r="V7" s="7">
+      <c r="P7" s="7">
+        <v>88.1</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R7" s="7">
+        <v>28.1</v>
+      </c>
+      <c r="S7" s="7">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T7" s="6">
+        <v>31.2</v>
+      </c>
+      <c r="U7" s="6">
+        <v>22</v>
+      </c>
+      <c r="V7" s="6">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="A8" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="B8" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="C8" s="5">
         <v>2.1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>5.0999999999999996</v>
       </c>
       <c r="E8" s="5">
@@ -1004,16 +1007,16 @@
       <c r="G8" s="4">
         <v>8.1</v>
       </c>
-      <c r="H8" s="3">
-        <v>9.1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="J8" s="5">
-        <v>11.1</v>
-      </c>
-      <c r="K8" s="5">
+      <c r="H8" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="K8" s="4">
         <v>12.1</v>
       </c>
       <c r="L8" s="7">
@@ -1043,7 +1046,7 @@
       <c r="T8" s="6">
         <v>31.2</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="6">
         <v>22</v>
       </c>
       <c r="V8" s="6">
@@ -1051,8 +1054,8 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>10.1</v>
+      <c r="A9" s="2">
+        <v>11.1</v>
       </c>
       <c r="B9" s="4">
         <v>1.1000000000000001</v>
@@ -1066,34 +1069,34 @@
       <c r="E9" s="5">
         <v>6.1</v>
       </c>
-      <c r="F9" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>8.1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>9.1</v>
-      </c>
-      <c r="I9" s="3">
-        <v>10.1</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="F9" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>8.1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>10.1</v>
+      </c>
+      <c r="J9" s="3">
         <v>11.1</v>
       </c>
       <c r="K9" s="4">
         <v>12.1</v>
       </c>
-      <c r="L9" s="7">
-        <v>86.1</v>
-      </c>
-      <c r="M9" s="7">
-        <v>35.1</v>
-      </c>
-      <c r="N9" s="7">
-        <v>26.1</v>
-      </c>
-      <c r="O9" s="7">
+      <c r="L9" s="6">
+        <v>86.1</v>
+      </c>
+      <c r="M9" s="6">
+        <v>35.1</v>
+      </c>
+      <c r="N9" s="6">
+        <v>26.1</v>
+      </c>
+      <c r="O9" s="6">
         <v>36.200000000000003</v>
       </c>
       <c r="P9" s="7">
@@ -1111,7 +1114,7 @@
       <c r="T9" s="6">
         <v>31.2</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="6">
         <v>22</v>
       </c>
       <c r="V9" s="6">
@@ -1119,8 +1122,8 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>11.1</v>
+      <c r="A10" s="2">
+        <v>12.1</v>
       </c>
       <c r="B10" s="4">
         <v>1.1000000000000001</v>
@@ -1128,13 +1131,13 @@
       <c r="C10" s="5">
         <v>2.1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>5.0999999999999996</v>
       </c>
       <c r="E10" s="5">
         <v>6.1</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>7.1</v>
       </c>
       <c r="G10" s="5">
@@ -1146,10 +1149,10 @@
       <c r="I10" s="4">
         <v>10.1</v>
       </c>
-      <c r="J10" s="3">
-        <v>11.1</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="J10" s="4">
+        <v>11.1</v>
+      </c>
+      <c r="K10" s="3">
         <v>12.1</v>
       </c>
       <c r="L10" s="6">
@@ -1176,87 +1179,87 @@
       <c r="S10" s="7">
         <v>38.200000000000003</v>
       </c>
-      <c r="T10" s="6">
-        <v>31.2</v>
-      </c>
-      <c r="U10" s="9">
-        <v>22</v>
-      </c>
-      <c r="V10" s="6">
+      <c r="T10" s="7">
+        <v>31.2</v>
+      </c>
+      <c r="U10" s="7">
+        <v>22</v>
+      </c>
+      <c r="V10" s="7">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>12.1</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2.1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E11" s="5">
-        <v>6.1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>8.1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>9.1</v>
-      </c>
-      <c r="I11" s="4">
-        <v>10.1</v>
-      </c>
-      <c r="J11" s="4">
-        <v>11.1</v>
-      </c>
-      <c r="K11" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="L11" s="6">
-        <v>86.1</v>
-      </c>
-      <c r="M11" s="6">
-        <v>35.1</v>
-      </c>
-      <c r="N11" s="6">
-        <v>26.1</v>
-      </c>
-      <c r="O11" s="6">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P11" s="7">
-        <v>88.1</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R11" s="7">
-        <v>28.1</v>
-      </c>
-      <c r="S11" s="7">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T11" s="7">
-        <v>31.2</v>
-      </c>
-      <c r="U11" s="8">
-        <v>22</v>
-      </c>
-      <c r="V11" s="7">
+      <c r="A11" s="2">
+        <v>86.1</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E11" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>9.1</v>
+      </c>
+      <c r="I11" s="7">
+        <v>10.1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>11.1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="L11" s="8">
+        <v>86.1</v>
+      </c>
+      <c r="M11" s="4">
+        <v>35.1</v>
+      </c>
+      <c r="N11" s="4">
+        <v>26.1</v>
+      </c>
+      <c r="O11" s="4">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P11" s="4">
+        <v>88.1</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R11" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="S11" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T11" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="U11" s="4">
+        <v>22</v>
+      </c>
+      <c r="V11" s="4">
         <v>32.200000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>86.1</v>
+      <c r="A12" s="2">
+        <v>35.1</v>
       </c>
       <c r="B12" s="6">
         <v>1.1000000000000001</v>
@@ -1288,10 +1291,10 @@
       <c r="K12" s="6">
         <v>12.1</v>
       </c>
-      <c r="L12" s="10">
-        <v>86.1</v>
-      </c>
-      <c r="M12" s="4">
+      <c r="L12" s="4">
+        <v>86.1</v>
+      </c>
+      <c r="M12" s="8">
         <v>35.1</v>
       </c>
       <c r="N12" s="4">
@@ -1315,7 +1318,7 @@
       <c r="T12" s="4">
         <v>31.2</v>
       </c>
-      <c r="U12" s="11">
+      <c r="U12" s="4">
         <v>22</v>
       </c>
       <c r="V12" s="4">
@@ -1323,8 +1326,8 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>35.1</v>
+      <c r="A13" s="2">
+        <v>26.1</v>
       </c>
       <c r="B13" s="6">
         <v>1.1000000000000001</v>
@@ -1359,10 +1362,10 @@
       <c r="L13" s="4">
         <v>86.1</v>
       </c>
-      <c r="M13" s="10">
-        <v>35.1</v>
-      </c>
-      <c r="N13" s="4">
+      <c r="M13" s="4">
+        <v>35.1</v>
+      </c>
+      <c r="N13" s="8">
         <v>26.1</v>
       </c>
       <c r="O13" s="4">
@@ -1383,7 +1386,7 @@
       <c r="T13" s="4">
         <v>31.2</v>
       </c>
-      <c r="U13" s="11">
+      <c r="U13" s="4">
         <v>22</v>
       </c>
       <c r="V13" s="4">
@@ -1391,8 +1394,8 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>26.1</v>
+      <c r="A14" s="2">
+        <v>36.1</v>
       </c>
       <c r="B14" s="6">
         <v>1.1000000000000001</v>
@@ -1430,10 +1433,10 @@
       <c r="M14" s="4">
         <v>35.1</v>
       </c>
-      <c r="N14" s="10">
-        <v>26.1</v>
-      </c>
-      <c r="O14" s="4">
+      <c r="N14" s="4">
+        <v>26.1</v>
+      </c>
+      <c r="O14" s="8">
         <v>36.200000000000003</v>
       </c>
       <c r="P14" s="4">
@@ -1451,7 +1454,7 @@
       <c r="T14" s="4">
         <v>31.2</v>
       </c>
-      <c r="U14" s="11">
+      <c r="U14" s="4">
         <v>22</v>
       </c>
       <c r="V14" s="4">
@@ -1459,25 +1462,25 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>36.1</v>
-      </c>
-      <c r="B15" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E15" s="7">
-        <v>6.1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>7.1</v>
-      </c>
-      <c r="G15" s="7">
+      <c r="A15" s="2">
+        <v>88.1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E15" s="6">
+        <v>6.1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7.1</v>
+      </c>
+      <c r="G15" s="6">
         <v>8.1</v>
       </c>
       <c r="H15" s="7">
@@ -1486,10 +1489,10 @@
       <c r="I15" s="7">
         <v>10.1</v>
       </c>
-      <c r="J15" s="6">
-        <v>11.1</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="J15" s="7">
+        <v>11.1</v>
+      </c>
+      <c r="K15" s="7">
         <v>12.1</v>
       </c>
       <c r="L15" s="4">
@@ -1501,10 +1504,10 @@
       <c r="N15" s="4">
         <v>26.1</v>
       </c>
-      <c r="O15" s="10">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P15" s="4">
+      <c r="O15" s="4">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P15" s="8">
         <v>88.1</v>
       </c>
       <c r="Q15" s="4">
@@ -1519,7 +1522,7 @@
       <c r="T15" s="4">
         <v>31.2</v>
       </c>
-      <c r="U15" s="11">
+      <c r="U15" s="4">
         <v>22</v>
       </c>
       <c r="V15" s="4">
@@ -1527,8 +1530,8 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>88.1</v>
+      <c r="A16" s="2">
+        <v>37.200000000000003</v>
       </c>
       <c r="B16" s="7">
         <v>1.1000000000000001</v>
@@ -1572,10 +1575,10 @@
       <c r="O16" s="4">
         <v>36.200000000000003</v>
       </c>
-      <c r="P16" s="10">
-        <v>88.1</v>
-      </c>
-      <c r="Q16" s="4">
+      <c r="P16" s="4">
+        <v>88.1</v>
+      </c>
+      <c r="Q16" s="8">
         <v>37.200000000000003</v>
       </c>
       <c r="R16" s="4">
@@ -1587,7 +1590,7 @@
       <c r="T16" s="4">
         <v>31.2</v>
       </c>
-      <c r="U16" s="11">
+      <c r="U16" s="4">
         <v>22</v>
       </c>
       <c r="V16" s="4">
@@ -1595,8 +1598,8 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>37.200000000000003</v>
+      <c r="A17" s="2">
+        <v>28.1</v>
       </c>
       <c r="B17" s="7">
         <v>1.1000000000000001</v>
@@ -1643,10 +1646,10 @@
       <c r="P17" s="4">
         <v>88.1</v>
       </c>
-      <c r="Q17" s="10">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R17" s="4">
+      <c r="Q17" s="4">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R17" s="8">
         <v>28.1</v>
       </c>
       <c r="S17" s="4">
@@ -1655,7 +1658,7 @@
       <c r="T17" s="4">
         <v>31.2</v>
       </c>
-      <c r="U17" s="11">
+      <c r="U17" s="4">
         <v>22</v>
       </c>
       <c r="V17" s="4">
@@ -1663,8 +1666,8 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>28.1</v>
+      <c r="A18" s="2">
+        <v>38.200000000000003</v>
       </c>
       <c r="B18" s="7">
         <v>1.1000000000000001</v>
@@ -1714,16 +1717,16 @@
       <c r="Q18" s="4">
         <v>37.200000000000003</v>
       </c>
-      <c r="R18" s="10">
-        <v>28.1</v>
-      </c>
-      <c r="S18" s="4">
+      <c r="R18" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="S18" s="8">
         <v>38.200000000000003</v>
       </c>
       <c r="T18" s="4">
         <v>31.2</v>
       </c>
-      <c r="U18" s="11">
+      <c r="U18" s="4">
         <v>22</v>
       </c>
       <c r="V18" s="4">
@@ -1731,13 +1734,13 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>38.200000000000003</v>
+      <c r="A19" s="2">
+        <v>32.1</v>
       </c>
       <c r="B19" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>2.1</v>
       </c>
       <c r="D19" s="7">
@@ -1749,16 +1752,16 @@
       <c r="F19" s="6">
         <v>7.1</v>
       </c>
-      <c r="G19" s="6">
-        <v>8.1</v>
-      </c>
-      <c r="H19" s="7">
-        <v>9.1</v>
-      </c>
-      <c r="I19" s="7">
-        <v>10.1</v>
-      </c>
-      <c r="J19" s="7">
+      <c r="G19" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="I19" s="6">
+        <v>10.1</v>
+      </c>
+      <c r="J19" s="6">
         <v>11.1</v>
       </c>
       <c r="K19" s="7">
@@ -1785,13 +1788,13 @@
       <c r="R19" s="4">
         <v>28.1</v>
       </c>
-      <c r="S19" s="10">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T19" s="4">
-        <v>31.2</v>
-      </c>
-      <c r="U19" s="11">
+      <c r="S19" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T19" s="8">
+        <v>31.2</v>
+      </c>
+      <c r="U19" s="4">
         <v>22</v>
       </c>
       <c r="V19" s="4">
@@ -1799,8 +1802,8 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>32.1</v>
+      <c r="A20" s="2">
+        <v>22</v>
       </c>
       <c r="B20" s="7">
         <v>1.1000000000000001</v>
@@ -1856,10 +1859,10 @@
       <c r="S20" s="4">
         <v>38.200000000000003</v>
       </c>
-      <c r="T20" s="10">
-        <v>31.2</v>
-      </c>
-      <c r="U20" s="11">
+      <c r="T20" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="U20" s="8">
         <v>22</v>
       </c>
       <c r="V20" s="4">
@@ -1867,8 +1870,8 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>22</v>
+      <c r="A21" s="2">
+        <v>32.200000000000003</v>
       </c>
       <c r="B21" s="7">
         <v>1.1000000000000001</v>
@@ -1927,78 +1930,10 @@
       <c r="T21" s="4">
         <v>31.2</v>
       </c>
-      <c r="U21" s="12">
-        <v>22</v>
-      </c>
-      <c r="V21" s="4">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2.1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E22" s="6">
-        <v>6.1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>7.1</v>
-      </c>
-      <c r="G22" s="7">
-        <v>8.1</v>
-      </c>
-      <c r="H22" s="6">
-        <v>9.1</v>
-      </c>
-      <c r="I22" s="6">
-        <v>10.1</v>
-      </c>
-      <c r="J22" s="6">
-        <v>11.1</v>
-      </c>
-      <c r="K22" s="7">
-        <v>12.1</v>
-      </c>
-      <c r="L22" s="4">
-        <v>86.1</v>
-      </c>
-      <c r="M22" s="4">
-        <v>35.1</v>
-      </c>
-      <c r="N22" s="4">
-        <v>26.1</v>
-      </c>
-      <c r="O22" s="4">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P22" s="4">
-        <v>88.1</v>
-      </c>
-      <c r="Q22" s="4">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R22" s="4">
-        <v>28.1</v>
-      </c>
-      <c r="S22" s="4">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T22" s="4">
-        <v>31.2</v>
-      </c>
-      <c r="U22" s="11">
-        <v>22</v>
-      </c>
-      <c r="V22" s="10">
+      <c r="U21" s="4">
+        <v>22</v>
+      </c>
+      <c r="V21" s="8">
         <v>32.200000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update conflict matrix and remove print statements
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.6.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerjan/Workshop/TrafficLightController/conflictMatrices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2895E-F961-AF4C-A374-52EA9CBD5F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AB9A9E-7506-44BE-B073-2484D1DEDF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="920" windowWidth="25040" windowHeight="13700" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +104,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -145,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -168,24 +183,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,18 +538,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -576,8 +616,26 @@
       <c r="V1" s="7">
         <v>32.200000000000003</v>
       </c>
+      <c r="W1" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X1" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y1" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z1" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA1" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB1" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2.1</v>
       </c>
@@ -644,8 +702,26 @@
       <c r="V2" s="7">
         <v>32.200000000000003</v>
       </c>
+      <c r="W2" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X2" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z2" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA2" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB2" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5.0999999999999996</v>
       </c>
@@ -712,8 +788,26 @@
       <c r="V3" s="7">
         <v>32.200000000000003</v>
       </c>
+      <c r="W3" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X3" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>6.1</v>
       </c>
@@ -780,8 +874,26 @@
       <c r="V4" s="6">
         <v>32.200000000000003</v>
       </c>
+      <c r="W4" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X4" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y4" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z4" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB4" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>7.1</v>
       </c>
@@ -848,8 +960,26 @@
       <c r="V5" s="6">
         <v>32.200000000000003</v>
       </c>
+      <c r="W5" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X5" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>8.1</v>
       </c>
@@ -916,8 +1046,26 @@
       <c r="V6" s="7">
         <v>32.200000000000003</v>
       </c>
+      <c r="W6" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X6" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB6" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.1</v>
       </c>
@@ -984,8 +1132,26 @@
       <c r="V7" s="6">
         <v>32.200000000000003</v>
       </c>
+      <c r="W7" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X7" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y7" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA7" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB7" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>10.1</v>
       </c>
@@ -1052,8 +1218,26 @@
       <c r="V8" s="6">
         <v>32.200000000000003</v>
       </c>
+      <c r="W8" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X8" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z8" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB8" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>11.1</v>
       </c>
@@ -1120,8 +1304,26 @@
       <c r="V9" s="6">
         <v>32.200000000000003</v>
       </c>
+      <c r="W9" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X9" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z9" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB9" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>12.1</v>
       </c>
@@ -1188,8 +1390,26 @@
       <c r="V10" s="7">
         <v>32.200000000000003</v>
       </c>
+      <c r="W10" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X10" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA10" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB10" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>86.1</v>
       </c>
@@ -1256,8 +1476,26 @@
       <c r="V11" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W11" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X11" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y11" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA11" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>35.1</v>
       </c>
@@ -1324,8 +1562,26 @@
       <c r="V12" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W12" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X12" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y12" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z12" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA12" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB12" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>26.1</v>
       </c>
@@ -1392,10 +1648,28 @@
       <c r="V13" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W13" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X13" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA13" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB13" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>36.1</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="B14" s="6">
         <v>1.1000000000000001</v>
@@ -1460,8 +1734,26 @@
       <c r="V14" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W14" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X14" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB14" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>88.1</v>
       </c>
@@ -1528,8 +1820,26 @@
       <c r="V15" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W15" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X15" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y15" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z15" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA15" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB15" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>37.200000000000003</v>
       </c>
@@ -1596,8 +1906,26 @@
       <c r="V16" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W16" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X16" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z16" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA16" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB16" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>28.1</v>
       </c>
@@ -1664,8 +1992,26 @@
       <c r="V17" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W17" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X17" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y17" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z17" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA17" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB17" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>38.200000000000003</v>
       </c>
@@ -1732,10 +2078,28 @@
       <c r="V18" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W18" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X18" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z18" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA18" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>32.1</v>
+        <v>31.2</v>
       </c>
       <c r="B19" s="7">
         <v>1.1000000000000001</v>
@@ -1800,8 +2164,26 @@
       <c r="V19" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W19" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X19" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y19" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z19" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA19" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB19" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>22</v>
       </c>
@@ -1868,8 +2250,26 @@
       <c r="V20" s="4">
         <v>32.200000000000003</v>
       </c>
+      <c r="W20" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X20" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z20" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA20" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>32.1</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>32.200000000000003</v>
       </c>
@@ -1935,6 +2335,540 @@
       </c>
       <c r="V21" s="8">
         <v>32.200000000000003</v>
+      </c>
+      <c r="W21" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X21" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y21" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z21" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA21" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB21" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D22" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E22" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G22" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H22" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I22" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J22" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K22" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L22" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M22" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N22" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O22" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P22" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R22" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S22" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T22" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U22" s="10">
+        <v>22</v>
+      </c>
+      <c r="V22" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W22" s="11">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X22" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y22" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z22" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA22" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB22" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>36.1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D23" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E23" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F23" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G23" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H23" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I23" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J23" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K23" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L23" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M23" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N23" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O23" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P23" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R23" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S23" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T23" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U23" s="10">
+        <v>22</v>
+      </c>
+      <c r="V23" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W23" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X23" s="11">
+        <v>36.1</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z23" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA23" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>37.1</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D24" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E24" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F24" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G24" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H24" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I24" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J24" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K24" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L24" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M24" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N24" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O24" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P24" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q24" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R24" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S24" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T24" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U24" s="10">
+        <v>22</v>
+      </c>
+      <c r="V24" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W24" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X24" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y24" s="11">
+        <v>37.1</v>
+      </c>
+      <c r="Z24" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA24" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB24" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>38.1</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D25" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E25" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G25" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H25" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I25" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J25" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K25" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L25" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M25" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N25" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O25" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P25" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q25" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R25" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S25" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T25" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U25" s="10">
+        <v>22</v>
+      </c>
+      <c r="V25" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W25" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X25" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y25" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z25" s="11">
+        <v>38.1</v>
+      </c>
+      <c r="AA25" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB25" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>31.1</v>
+      </c>
+      <c r="B26" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E26" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G26" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H26" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I26" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J26" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K26" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L26" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M26" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N26" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O26" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P26" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R26" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S26" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T26" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U26" s="10">
+        <v>22</v>
+      </c>
+      <c r="V26" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W26" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X26" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y26" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z26" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA26" s="11">
+        <v>31.1</v>
+      </c>
+      <c r="AB26" s="10">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>32.1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="D27" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E27" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="G27" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="H27" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="J27" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K27" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="L27" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="M27" s="10">
+        <v>35.1</v>
+      </c>
+      <c r="N27" s="10">
+        <v>26.1</v>
+      </c>
+      <c r="O27" s="10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="P27" s="10">
+        <v>88.1</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="R27" s="10">
+        <v>28.1</v>
+      </c>
+      <c r="S27" s="10">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="T27" s="10">
+        <v>31.2</v>
+      </c>
+      <c r="U27" s="10">
+        <v>22</v>
+      </c>
+      <c r="V27" s="10">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="W27" s="10">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="X27" s="10">
+        <v>36.1</v>
+      </c>
+      <c r="Y27" s="10">
+        <v>37.1</v>
+      </c>
+      <c r="Z27" s="10">
+        <v>38.1</v>
+      </c>
+      <c r="AA27" s="10">
+        <v>31.1</v>
+      </c>
+      <c r="AB27" s="11">
+        <v>32.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>